<commit_message>
Final project Camera last commit
</commit_message>
<xml_diff>
--- a/Camera/2DFeature_Matching/perfEval2.xlsx
+++ b/Camera/2DFeature_Matching/perfEval2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KHIM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KHIM\Desktop\Udacity_Sensor_Fusion_Eng\Camera\2DFeature_Matching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6D5C42-1040-4DB3-ADAB-598222E731BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5914D29F-3D39-4050-AE31-C8D8E480B529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1249,14 +1249,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1264,7 +1264,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1581,28 +1580,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F204" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
+      <selection activeCell="N213" sqref="N213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" customWidth="1"/>
-    <col min="17" max="17" width="15.77734375" customWidth="1"/>
-    <col min="18" max="18" width="14.88671875" customWidth="1"/>
-    <col min="19" max="19" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1616,7 @@
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>13</v>
       </c>
@@ -1645,7 +1644,7 @@
         <v>41.7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>14</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>15</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>19.36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>16</v>
       </c>
@@ -1687,7 +1686,7 @@
         <v>13.23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>17</v>
       </c>
@@ -1701,7 +1700,7 @@
         <v>12.59</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>18</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>11.88</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>19</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>13.61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>20</v>
       </c>
@@ -1743,7 +1742,7 @@
         <v>11.86</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>21</v>
       </c>
@@ -1757,7 +1756,7 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>22</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>11.74</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G13" s="1" t="s">
         <v>222</v>
       </c>
@@ -1784,7 +1783,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>13</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>22.78</v>
       </c>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>14</v>
       </c>
@@ -1812,7 +1811,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>15</v>
       </c>
@@ -1826,7 +1825,7 @@
         <v>19.79</v>
       </c>
     </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>16</v>
       </c>
@@ -1840,7 +1839,7 @@
         <v>14.63</v>
       </c>
     </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>17</v>
       </c>
@@ -1854,7 +1853,7 @@
         <v>15.12</v>
       </c>
     </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>18</v>
       </c>
@@ -1868,7 +1867,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>19</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>13.39</v>
       </c>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>20</v>
       </c>
@@ -1896,7 +1895,7 @@
         <v>15.79</v>
       </c>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>21</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>14.81</v>
       </c>
     </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>22</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>19.649999999999999</v>
       </c>
     </row>
-    <row r="26" spans="6:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G26" s="1" t="s">
         <v>222</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>18.706</v>
       </c>
     </row>
-    <row r="29" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>13</v>
       </c>
@@ -1951,7 +1950,7 @@
         <v>182.43</v>
       </c>
     </row>
-    <row r="30" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>14</v>
       </c>
@@ -1965,7 +1964,7 @@
         <v>160.97999999999999</v>
       </c>
     </row>
-    <row r="31" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>15</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>172.69</v>
       </c>
     </row>
-    <row r="32" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>16</v>
       </c>
@@ -1993,7 +1992,7 @@
         <v>160.53</v>
       </c>
     </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>17</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v>163.94</v>
       </c>
     </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>18</v>
       </c>
@@ -2021,7 +2020,7 @@
         <v>162.47999999999999</v>
       </c>
     </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>19</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>164.29</v>
       </c>
     </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>20</v>
       </c>
@@ -2049,7 +2048,7 @@
         <v>162.79</v>
       </c>
     </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>21</v>
       </c>
@@ -2063,7 +2062,7 @@
         <v>167.54</v>
       </c>
     </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>22</v>
       </c>
@@ -2077,7 +2076,7 @@
         <v>163.55000000000001</v>
       </c>
     </row>
-    <row r="39" spans="6:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G39" s="1" t="s">
         <v>222</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>166.12199999999999</v>
       </c>
     </row>
-    <row r="42" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>13</v>
       </c>
@@ -2104,7 +2103,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="43" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>14</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="44" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>15</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="45" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>16</v>
       </c>
@@ -2146,7 +2145,7 @@
         <v>2.82</v>
       </c>
     </row>
-    <row r="46" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>17</v>
       </c>
@@ -2160,7 +2159,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="47" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>18</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="48" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>19</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="49" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
         <v>20</v>
       </c>
@@ -2202,7 +2201,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="50" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
         <v>21</v>
       </c>
@@ -2216,7 +2215,7 @@
         <v>2.82</v>
       </c>
     </row>
-    <row r="51" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
         <v>22</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="52" spans="6:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G52" s="1" t="s">
         <v>222</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>3.0419999999999998</v>
       </c>
     </row>
-    <row r="55" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
         <v>13</v>
       </c>
@@ -2257,7 +2256,7 @@
         <v>52.07</v>
       </c>
     </row>
-    <row r="56" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
         <v>14</v>
       </c>
@@ -2271,7 +2270,7 @@
         <v>51.01</v>
       </c>
     </row>
-    <row r="57" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
         <v>15</v>
       </c>
@@ -2285,7 +2284,7 @@
         <v>49.43</v>
       </c>
     </row>
-    <row r="58" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
         <v>16</v>
       </c>
@@ -2299,7 +2298,7 @@
         <v>47.63</v>
       </c>
     </row>
-    <row r="59" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
         <v>17</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>47.56</v>
       </c>
     </row>
-    <row r="60" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
         <v>18</v>
       </c>
@@ -2327,7 +2326,7 @@
         <v>48.07</v>
       </c>
     </row>
-    <row r="61" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
         <v>19</v>
       </c>
@@ -2341,7 +2340,7 @@
         <v>47.73</v>
       </c>
     </row>
-    <row r="62" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
         <v>20</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>47.28</v>
       </c>
     </row>
-    <row r="63" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
         <v>21</v>
       </c>
@@ -2369,7 +2368,7 @@
         <v>47.33</v>
       </c>
     </row>
-    <row r="64" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
         <v>22</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>47.44</v>
       </c>
     </row>
-    <row r="65" spans="6:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G65" s="1" t="s">
         <v>222</v>
       </c>
@@ -2396,7 +2395,7 @@
         <v>48.554999999999993</v>
       </c>
     </row>
-    <row r="68" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
         <v>13</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>18.45</v>
       </c>
     </row>
-    <row r="69" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
         <v>14</v>
       </c>
@@ -2424,7 +2423,7 @@
         <v>9.51</v>
       </c>
     </row>
-    <row r="70" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
         <v>15</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="71" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
         <v>16</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="72" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
         <v>17</v>
       </c>
@@ -2466,7 +2465,7 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="73" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
         <v>18</v>
       </c>
@@ -2480,7 +2479,7 @@
         <v>7.77</v>
       </c>
     </row>
-    <row r="74" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
         <v>19</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="75" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
         <v>20</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>8.8699999999999992</v>
       </c>
     </row>
-    <row r="76" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>21</v>
       </c>
@@ -2522,7 +2521,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="77" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F77" t="s">
         <v>22</v>
       </c>
@@ -2536,7 +2535,7 @@
         <v>7.72</v>
       </c>
     </row>
-    <row r="78" spans="6:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G78" s="1" t="s">
         <v>222</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>9.1610000000000014</v>
       </c>
     </row>
-    <row r="81" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
         <v>13</v>
       </c>
@@ -2563,7 +2562,7 @@
         <v>126.38</v>
       </c>
     </row>
-    <row r="82" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
         <v>14</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>111.27</v>
       </c>
     </row>
-    <row r="83" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
         <v>15</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>119.69</v>
       </c>
     </row>
-    <row r="84" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
         <v>16</v>
       </c>
@@ -2605,7 +2604,7 @@
         <v>113.45</v>
       </c>
     </row>
-    <row r="85" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
         <v>17</v>
       </c>
@@ -2619,7 +2618,7 @@
         <v>117.29</v>
       </c>
     </row>
-    <row r="86" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
         <v>18</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>112.18</v>
       </c>
     </row>
-    <row r="87" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
         <v>19</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>110.12</v>
       </c>
     </row>
-    <row r="88" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
         <v>20</v>
       </c>
@@ -2661,7 +2660,7 @@
         <v>116.04</v>
       </c>
     </row>
-    <row r="89" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
         <v>21</v>
       </c>
@@ -2675,7 +2674,7 @@
         <v>119.59</v>
       </c>
     </row>
-    <row r="90" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F90" t="s">
         <v>22</v>
       </c>
@@ -2689,7 +2688,7 @@
         <v>115.02</v>
       </c>
     </row>
-    <row r="91" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G91" s="1" t="s">
         <v>222</v>
       </c>
@@ -2702,17 +2701,17 @@
         <v>116.10299999999999</v>
       </c>
     </row>
-    <row r="94" spans="6:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="H94" s="10"/>
-      <c r="I94" s="10"/>
-      <c r="J94" s="10"/>
-    </row>
-    <row r="95" spans="6:12" ht="21" x14ac:dyDescent="0.4">
-      <c r="H95" s="10"/>
-      <c r="I95" s="10"/>
-      <c r="J95" s="10"/>
-    </row>
-    <row r="96" spans="6:12" ht="22.2" x14ac:dyDescent="0.45">
+    <row r="94" spans="6:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+    </row>
+    <row r="95" spans="6:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+    </row>
+    <row r="96" spans="6:12" ht="22.5" x14ac:dyDescent="0.35">
       <c r="F96" s="8" t="s">
         <v>255</v>
       </c>
@@ -2723,7 +2722,7 @@
       <c r="K96" s="8"/>
       <c r="L96" s="8"/>
     </row>
-    <row r="97" spans="6:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="97" spans="6:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F97" s="1" t="s">
         <v>1</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="98" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
         <v>13</v>
       </c>
@@ -2760,14 +2759,14 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="99" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F99" t="s">
         <v>14</v>
       </c>
       <c r="G99" t="s">
         <v>12</v>
       </c>
-      <c r="H99" s="5" t="s">
+      <c r="H99" t="s">
         <v>25</v>
       </c>
       <c r="I99">
@@ -2780,14 +2779,14 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="100" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F100" t="s">
         <v>15</v>
       </c>
       <c r="G100" t="s">
         <v>12</v>
       </c>
-      <c r="H100" s="5" t="s">
+      <c r="H100" t="s">
         <v>29</v>
       </c>
       <c r="I100">
@@ -2800,14 +2799,14 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="101" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F101" t="s">
         <v>16</v>
       </c>
       <c r="G101" t="s">
         <v>12</v>
       </c>
-      <c r="H101" s="5" t="s">
+      <c r="H101" t="s">
         <v>30</v>
       </c>
       <c r="I101">
@@ -2820,14 +2819,14 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="102" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F102" t="s">
         <v>17</v>
       </c>
       <c r="G102" t="s">
         <v>12</v>
       </c>
-      <c r="H102" s="5" t="s">
+      <c r="H102" t="s">
         <v>31</v>
       </c>
       <c r="I102">
@@ -2840,14 +2839,14 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="103" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F103" t="s">
         <v>18</v>
       </c>
       <c r="G103" t="s">
         <v>12</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H103" t="s">
         <v>32</v>
       </c>
       <c r="I103">
@@ -2860,14 +2859,14 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="104" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F104" t="s">
         <v>19</v>
       </c>
       <c r="G104" t="s">
         <v>12</v>
       </c>
-      <c r="H104" s="5" t="s">
+      <c r="H104" t="s">
         <v>33</v>
       </c>
       <c r="I104">
@@ -2880,14 +2879,14 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="105" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F105" t="s">
         <v>20</v>
       </c>
       <c r="G105" t="s">
         <v>12</v>
       </c>
-      <c r="H105" s="5" t="s">
+      <c r="H105" t="s">
         <v>34</v>
       </c>
       <c r="I105">
@@ -2900,14 +2899,14 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="106" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F106" t="s">
         <v>21</v>
       </c>
       <c r="G106" t="s">
         <v>12</v>
       </c>
-      <c r="H106" s="5" t="s">
+      <c r="H106" t="s">
         <v>35</v>
       </c>
       <c r="I106">
@@ -2920,14 +2919,14 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="107" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F107" t="s">
         <v>22</v>
       </c>
       <c r="G107" t="s">
         <v>12</v>
       </c>
-      <c r="H107" s="5" t="s">
+      <c r="H107" t="s">
         <v>36</v>
       </c>
       <c r="I107">
@@ -2940,7 +2939,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="108" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G108" s="1" t="s">
         <v>222</v>
       </c>
@@ -2957,7 +2956,7 @@
         <v>20.437999999999999</v>
       </c>
     </row>
-    <row r="111" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
         <v>13</v>
       </c>
@@ -2971,14 +2970,14 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="112" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F112" t="s">
         <v>14</v>
       </c>
       <c r="G112" t="s">
         <v>37</v>
       </c>
-      <c r="H112" s="5" t="s">
+      <c r="H112" t="s">
         <v>38</v>
       </c>
       <c r="I112">
@@ -2991,14 +2990,14 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="113" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F113" t="s">
         <v>15</v>
       </c>
       <c r="G113" t="s">
         <v>37</v>
       </c>
-      <c r="H113" s="5" t="s">
+      <c r="H113" t="s">
         <v>39</v>
       </c>
       <c r="I113">
@@ -3011,14 +3010,14 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="114" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F114" t="s">
         <v>16</v>
       </c>
       <c r="G114" t="s">
         <v>37</v>
       </c>
-      <c r="H114" s="5" t="s">
+      <c r="H114" t="s">
         <v>40</v>
       </c>
       <c r="I114">
@@ -3031,14 +3030,14 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="115" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F115" t="s">
         <v>17</v>
       </c>
       <c r="G115" t="s">
         <v>37</v>
       </c>
-      <c r="H115" s="5" t="s">
+      <c r="H115" t="s">
         <v>41</v>
       </c>
       <c r="I115">
@@ -3051,14 +3050,14 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="116" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F116" t="s">
         <v>18</v>
       </c>
       <c r="G116" t="s">
         <v>37</v>
       </c>
-      <c r="H116" s="5" t="s">
+      <c r="H116" t="s">
         <v>42</v>
       </c>
       <c r="I116">
@@ -3071,14 +3070,14 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="117" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F117" t="s">
         <v>19</v>
       </c>
       <c r="G117" t="s">
         <v>37</v>
       </c>
-      <c r="H117" s="5" t="s">
+      <c r="H117" t="s">
         <v>30</v>
       </c>
       <c r="I117">
@@ -3091,14 +3090,14 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="118" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F118" t="s">
         <v>20</v>
       </c>
       <c r="G118" t="s">
         <v>37</v>
       </c>
-      <c r="H118" s="5" t="s">
+      <c r="H118" t="s">
         <v>43</v>
       </c>
       <c r="I118">
@@ -3111,14 +3110,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F119" t="s">
         <v>21</v>
       </c>
       <c r="G119" t="s">
         <v>37</v>
       </c>
-      <c r="H119" s="5" t="s">
+      <c r="H119" t="s">
         <v>30</v>
       </c>
       <c r="I119">
@@ -3131,14 +3130,14 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="120" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F120" t="s">
         <v>22</v>
       </c>
       <c r="G120" t="s">
         <v>37</v>
       </c>
-      <c r="H120" s="5" t="s">
+      <c r="H120" t="s">
         <v>43</v>
       </c>
       <c r="I120">
@@ -3151,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G121" s="1" t="s">
         <v>222</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>19.530999999999999</v>
       </c>
     </row>
-    <row r="124" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F124" t="s">
         <v>13</v>
       </c>
@@ -3182,7 +3181,7 @@
         <v>51.27</v>
       </c>
     </row>
-    <row r="125" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F125" t="s">
         <v>14</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>47.48</v>
       </c>
     </row>
-    <row r="126" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F126" t="s">
         <v>15</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="127" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F127" t="s">
         <v>16</v>
       </c>
@@ -3242,7 +3241,7 @@
         <v>48.95</v>
       </c>
     </row>
-    <row r="128" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F128" t="s">
         <v>17</v>
       </c>
@@ -3262,7 +3261,7 @@
         <v>49.67</v>
       </c>
     </row>
-    <row r="129" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F129" t="s">
         <v>18</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>48.87</v>
       </c>
     </row>
-    <row r="130" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F130" t="s">
         <v>19</v>
       </c>
@@ -3302,7 +3301,7 @@
         <v>48.79</v>
       </c>
     </row>
-    <row r="131" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F131" t="s">
         <v>20</v>
       </c>
@@ -3322,7 +3321,7 @@
         <v>49.41</v>
       </c>
     </row>
-    <row r="132" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F132" t="s">
         <v>21</v>
       </c>
@@ -3342,7 +3341,7 @@
         <v>48.89</v>
       </c>
     </row>
-    <row r="133" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F133" t="s">
         <v>22</v>
       </c>
@@ -3362,7 +3361,7 @@
         <v>48.8</v>
       </c>
     </row>
-    <row r="134" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G134" s="1" t="s">
         <v>222</v>
       </c>
@@ -3379,7 +3378,7 @@
         <v>63.352000000000004</v>
       </c>
     </row>
-    <row r="137" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F137" t="s">
         <v>13</v>
       </c>
@@ -3393,7 +3392,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="138" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F138" t="s">
         <v>14</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>17.170000000000002</v>
       </c>
     </row>
-    <row r="139" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F139" t="s">
         <v>15</v>
       </c>
@@ -3433,7 +3432,7 @@
         <v>23.12</v>
       </c>
     </row>
-    <row r="140" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F140" t="s">
         <v>16</v>
       </c>
@@ -3453,7 +3452,7 @@
         <v>18.07</v>
       </c>
     </row>
-    <row r="141" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F141" t="s">
         <v>17</v>
       </c>
@@ -3473,7 +3472,7 @@
         <v>18.72</v>
       </c>
     </row>
-    <row r="142" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F142" t="s">
         <v>18</v>
       </c>
@@ -3493,7 +3492,7 @@
         <v>24.53</v>
       </c>
     </row>
-    <row r="143" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F143" t="s">
         <v>19</v>
       </c>
@@ -3513,7 +3512,7 @@
         <v>21.09</v>
       </c>
     </row>
-    <row r="144" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F144" t="s">
         <v>20</v>
       </c>
@@ -3533,7 +3532,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="145" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F145" t="s">
         <v>21</v>
       </c>
@@ -3553,7 +3552,7 @@
         <v>21.66</v>
       </c>
     </row>
-    <row r="146" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F146" t="s">
         <v>22</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>20.27</v>
       </c>
     </row>
-    <row r="147" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G147" s="1" t="s">
         <v>222</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>36.322000000000003</v>
       </c>
     </row>
-    <row r="150" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F150" t="s">
         <v>13</v>
       </c>
@@ -3604,7 +3603,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="151" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F151" t="s">
         <v>14</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="152" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F152" t="s">
         <v>15</v>
       </c>
@@ -3644,7 +3643,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="153" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F153" t="s">
         <v>16</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="154" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F154" t="s">
         <v>17</v>
       </c>
@@ -3684,7 +3683,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="155" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F155" t="s">
         <v>18</v>
       </c>
@@ -3704,7 +3703,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="156" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F156" t="s">
         <v>19</v>
       </c>
@@ -3724,7 +3723,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="157" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F157" t="s">
         <v>20</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="158" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F158" t="s">
         <v>21</v>
       </c>
@@ -3764,7 +3763,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="159" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F159" t="s">
         <v>22</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="160" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G160" s="1" t="s">
         <v>222</v>
       </c>
@@ -3801,7 +3800,7 @@
         <v>23.054000000000006</v>
       </c>
     </row>
-    <row r="163" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F163" t="s">
         <v>13</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="164" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F164" t="s">
         <v>14</v>
       </c>
@@ -3835,7 +3834,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="165" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F165" t="s">
         <v>15</v>
       </c>
@@ -3855,7 +3854,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="166" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F166" t="s">
         <v>16</v>
       </c>
@@ -3875,7 +3874,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="167" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F167" t="s">
         <v>17</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="168" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F168" t="s">
         <v>18</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="169" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F169" t="s">
         <v>19</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="170" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F170" t="s">
         <v>20</v>
       </c>
@@ -3955,7 +3954,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="171" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F171" t="s">
         <v>21</v>
       </c>
@@ -3975,7 +3974,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="172" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F172" t="s">
         <v>22</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="173" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="173" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G173" s="1" t="s">
         <v>222</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>26.635999999999996</v>
       </c>
     </row>
-    <row r="176" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F176" t="s">
         <v>13</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>55.87</v>
       </c>
     </row>
-    <row r="177" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F177" t="s">
         <v>14</v>
       </c>
@@ -4046,7 +4045,7 @@
         <v>47.69</v>
       </c>
     </row>
-    <row r="178" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F178" t="s">
         <v>15</v>
       </c>
@@ -4066,7 +4065,7 @@
         <v>49.56</v>
       </c>
     </row>
-    <row r="179" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F179" t="s">
         <v>16</v>
       </c>
@@ -4086,7 +4085,7 @@
         <v>48.72</v>
       </c>
     </row>
-    <row r="180" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F180" t="s">
         <v>17</v>
       </c>
@@ -4106,7 +4105,7 @@
         <v>50.51</v>
       </c>
     </row>
-    <row r="181" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F181" t="s">
         <v>18</v>
       </c>
@@ -4126,7 +4125,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="182" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F182" t="s">
         <v>19</v>
       </c>
@@ -4146,7 +4145,7 @@
         <v>48.79</v>
       </c>
     </row>
-    <row r="183" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F183" t="s">
         <v>20</v>
       </c>
@@ -4166,7 +4165,7 @@
         <v>48.2</v>
       </c>
     </row>
-    <row r="184" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F184" t="s">
         <v>21</v>
       </c>
@@ -4186,7 +4185,7 @@
         <v>48.4</v>
       </c>
     </row>
-    <row r="185" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F185" t="s">
         <v>22</v>
       </c>
@@ -4206,7 +4205,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="186" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G186" s="1" t="s">
         <v>222</v>
       </c>
@@ -4223,7 +4222,7 @@
         <v>68.784999999999997</v>
       </c>
     </row>
-    <row r="189" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F189" t="s">
         <v>13</v>
       </c>
@@ -4237,7 +4236,7 @@
         <v>29.86</v>
       </c>
     </row>
-    <row r="190" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F190" t="s">
         <v>14</v>
       </c>
@@ -4257,7 +4256,7 @@
         <v>18.64</v>
       </c>
     </row>
-    <row r="191" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F191" t="s">
         <v>15</v>
       </c>
@@ -4277,7 +4276,7 @@
         <v>26.52</v>
       </c>
     </row>
-    <row r="192" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F192" t="s">
         <v>16</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>25.38</v>
       </c>
     </row>
-    <row r="193" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="193" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F193" t="s">
         <v>17</v>
       </c>
@@ -4317,7 +4316,7 @@
         <v>20.25</v>
       </c>
     </row>
-    <row r="194" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="194" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F194" t="s">
         <v>18</v>
       </c>
@@ -4337,7 +4336,7 @@
         <v>27.82</v>
       </c>
     </row>
-    <row r="195" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="195" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F195" t="s">
         <v>19</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>27.63</v>
       </c>
     </row>
-    <row r="196" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="196" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F196" t="s">
         <v>20</v>
       </c>
@@ -4377,7 +4376,7 @@
         <v>29.74</v>
       </c>
     </row>
-    <row r="197" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="197" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F197" t="s">
         <v>21</v>
       </c>
@@ -4397,7 +4396,7 @@
         <v>25.89</v>
       </c>
     </row>
-    <row r="198" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="198" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F198" t="s">
         <v>22</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>25.14</v>
       </c>
     </row>
-    <row r="199" spans="6:19" ht="21" x14ac:dyDescent="0.4">
+    <row r="199" spans="6:19" ht="21" x14ac:dyDescent="0.35">
       <c r="G199" s="1" t="s">
         <v>222</v>
       </c>
@@ -4433,17 +4432,17 @@
         <f>SUM(J199:K199)</f>
         <v>48.305999999999997</v>
       </c>
-      <c r="P199" s="10" t="s">
+      <c r="P199" s="6" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="200" spans="6:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="N200" s="6" t="s">
+    <row r="200" spans="6:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N200" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="201" spans="6:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="G201" s="6" t="s">
+    <row r="201" spans="6:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G201" s="5" t="s">
         <v>251</v>
       </c>
       <c r="N201" s="1" t="s">
@@ -4465,7 +4464,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="202" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="202" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F202" t="s">
         <v>13</v>
       </c>
@@ -4491,7 +4490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="203" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F203" t="s">
         <v>14</v>
       </c>
@@ -4526,7 +4525,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="204" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="204" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F204" t="s">
         <v>15</v>
       </c>
@@ -4561,7 +4560,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="205" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="205" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F205" t="s">
         <v>16</v>
       </c>
@@ -4596,7 +4595,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="206" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="206" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F206" t="s">
         <v>17</v>
       </c>
@@ -4631,7 +4630,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="207" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="207" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F207" t="s">
         <v>18</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="208" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="208" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F208" t="s">
         <v>19</v>
       </c>
@@ -4701,7 +4700,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="209" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="209" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F209" t="s">
         <v>20</v>
       </c>
@@ -4736,7 +4735,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="210" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="210" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F210" t="s">
         <v>21</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="211" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="211" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F211" t="s">
         <v>22</v>
       </c>
@@ -4806,7 +4805,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="212" spans="6:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="212" spans="6:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G212" s="1" t="s">
         <v>222</v>
       </c>
@@ -4825,7 +4824,7 @@
       <c r="O212" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="P212" s="5">
+      <c r="P212">
         <f>AVERAGE(P203:P211)</f>
         <v>81.777777777777771</v>
       </c>
@@ -4842,13 +4841,13 @@
         <v>3.7109999999999999</v>
       </c>
     </row>
-    <row r="213" spans="6:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="N213" s="6" t="s">
+    <row r="213" spans="6:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N213" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="214" spans="6:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="G214" s="6" t="s">
+    <row r="214" spans="6:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G214" s="5" t="s">
         <v>250</v>
       </c>
       <c r="N214" s="1" t="s">
@@ -4871,7 +4870,7 @@
       </c>
       <c r="T214" s="1"/>
     </row>
-    <row r="215" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="215" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F215" t="s">
         <v>13</v>
       </c>
@@ -4897,7 +4896,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="216" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="216" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F216" t="s">
         <v>14</v>
       </c>
@@ -4932,7 +4931,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="217" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="217" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F217" t="s">
         <v>15</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="218" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="218" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F218" t="s">
         <v>16</v>
       </c>
@@ -5002,7 +5001,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="219" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="219" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F219" t="s">
         <v>17</v>
       </c>
@@ -5037,7 +5036,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="220" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="220" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F220" t="s">
         <v>18</v>
       </c>
@@ -5072,7 +5071,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="221" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="221" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F221" t="s">
         <v>19</v>
       </c>
@@ -5107,7 +5106,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="222" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="222" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F222" t="s">
         <v>20</v>
       </c>
@@ -5142,7 +5141,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="223" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="223" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F223" t="s">
         <v>21</v>
       </c>
@@ -5177,7 +5176,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="224" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="224" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F224" t="s">
         <v>22</v>
       </c>
@@ -5212,7 +5211,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="225" spans="6:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="225" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G225" s="1" t="s">
         <v>222</v>
       </c>
@@ -5248,7 +5247,7 @@
         <v>4.2949999999999999</v>
       </c>
     </row>
-    <row r="228" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="228" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F228" t="s">
         <v>13</v>
       </c>
@@ -5262,7 +5261,7 @@
         <v>56.3</v>
       </c>
     </row>
-    <row r="229" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="229" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F229" t="s">
         <v>14</v>
       </c>
@@ -5282,7 +5281,7 @@
         <v>55.6</v>
       </c>
     </row>
-    <row r="230" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="230" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F230" t="s">
         <v>15</v>
       </c>
@@ -5302,7 +5301,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="231" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="231" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F231" t="s">
         <v>16</v>
       </c>
@@ -5322,7 +5321,7 @@
         <v>51.3</v>
       </c>
     </row>
-    <row r="232" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="232" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F232" t="s">
         <v>17</v>
       </c>
@@ -5342,7 +5341,7 @@
         <v>50.89</v>
       </c>
     </row>
-    <row r="233" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="233" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F233" t="s">
         <v>18</v>
       </c>
@@ -5362,7 +5361,7 @@
         <v>49.26</v>
       </c>
     </row>
-    <row r="234" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="234" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F234" t="s">
         <v>19</v>
       </c>
@@ -5382,7 +5381,7 @@
         <v>50.42</v>
       </c>
     </row>
-    <row r="235" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="235" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F235" t="s">
         <v>20</v>
       </c>
@@ -5402,7 +5401,7 @@
         <v>51.04</v>
       </c>
     </row>
-    <row r="236" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="236" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F236" t="s">
         <v>21</v>
       </c>
@@ -5422,7 +5421,7 @@
         <v>50.66</v>
       </c>
     </row>
-    <row r="237" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="237" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F237" t="s">
         <v>22</v>
       </c>
@@ -5442,7 +5441,7 @@
         <v>52.02</v>
       </c>
     </row>
-    <row r="238" spans="6:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="238" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G238" s="1" t="s">
         <v>222</v>
       </c>
@@ -5459,7 +5458,7 @@
         <v>55.725999999999999</v>
       </c>
     </row>
-    <row r="241" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F241" t="s">
         <v>13</v>
       </c>
@@ -5473,7 +5472,7 @@
         <v>46.46</v>
       </c>
     </row>
-    <row r="242" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="242" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F242" t="s">
         <v>14</v>
       </c>
@@ -5493,7 +5492,7 @@
         <v>44.79</v>
       </c>
     </row>
-    <row r="243" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="243" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F243" t="s">
         <v>15</v>
       </c>
@@ -5513,7 +5512,7 @@
         <v>41.87</v>
       </c>
     </row>
-    <row r="244" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="244" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F244" t="s">
         <v>16</v>
       </c>
@@ -5533,7 +5532,7 @@
         <v>26.77</v>
       </c>
     </row>
-    <row r="245" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="245" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F245" t="s">
         <v>17</v>
       </c>
@@ -5553,7 +5552,7 @@
         <v>38.85</v>
       </c>
     </row>
-    <row r="246" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="246" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F246" t="s">
         <v>18</v>
       </c>
@@ -5573,7 +5572,7 @@
         <v>33.32</v>
       </c>
     </row>
-    <row r="247" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="247" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F247" t="s">
         <v>19</v>
       </c>
@@ -5593,7 +5592,7 @@
         <v>32.71</v>
       </c>
     </row>
-    <row r="248" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="248" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F248" t="s">
         <v>20</v>
       </c>
@@ -5613,7 +5612,7 @@
         <v>38.07</v>
       </c>
     </row>
-    <row r="249" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="249" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F249" t="s">
         <v>21</v>
       </c>
@@ -5633,7 +5632,7 @@
         <v>37.04</v>
       </c>
     </row>
-    <row r="250" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="250" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F250" t="s">
         <v>22</v>
       </c>
@@ -5653,7 +5652,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="251" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="251" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G251" s="1" t="s">
         <v>222</v>
       </c>
@@ -5670,7 +5669,7 @@
         <v>40.526999999999994</v>
       </c>
     </row>
-    <row r="254" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="254" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F254" t="s">
         <v>13</v>
       </c>
@@ -5684,7 +5683,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="255" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F255" t="s">
         <v>14</v>
       </c>
@@ -5704,7 +5703,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="256" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F256" t="s">
         <v>15</v>
       </c>
@@ -5724,7 +5723,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="257" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="257" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F257" t="s">
         <v>16</v>
       </c>
@@ -5744,7 +5743,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="258" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F258" t="s">
         <v>17</v>
       </c>
@@ -5764,7 +5763,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="259" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="259" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F259" t="s">
         <v>18</v>
       </c>
@@ -5784,7 +5783,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="260" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="260" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F260" t="s">
         <v>19</v>
       </c>
@@ -5804,7 +5803,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="261" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="261" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F261" t="s">
         <v>20</v>
       </c>
@@ -5824,7 +5823,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="262" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="262" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F262" t="s">
         <v>21</v>
       </c>
@@ -5844,7 +5843,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="263" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="263" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F263" t="s">
         <v>22</v>
       </c>
@@ -5864,7 +5863,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="264" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G264" s="1" t="s">
         <v>222</v>
       </c>
@@ -5881,7 +5880,7 @@
         <v>51.122</v>
       </c>
     </row>
-    <row r="267" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="267" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F267" t="s">
         <v>13</v>
       </c>
@@ -5895,7 +5894,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="268" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="268" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F268" t="s">
         <v>14</v>
       </c>
@@ -5915,7 +5914,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="269" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="269" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F269" t="s">
         <v>15</v>
       </c>
@@ -5935,7 +5934,7 @@
         <v>5.23</v>
       </c>
     </row>
-    <row r="270" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="270" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F270" t="s">
         <v>16</v>
       </c>
@@ -5955,7 +5954,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="271" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="271" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F271" t="s">
         <v>17</v>
       </c>
@@ -5975,7 +5974,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="272" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="272" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F272" t="s">
         <v>18</v>
       </c>
@@ -5995,7 +5994,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="273" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F273" t="s">
         <v>19</v>
       </c>
@@ -6015,7 +6014,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="274" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F274" t="s">
         <v>20</v>
       </c>
@@ -6035,7 +6034,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="275" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F275" t="s">
         <v>21</v>
       </c>
@@ -6055,7 +6054,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="276" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F276" t="s">
         <v>22</v>
       </c>
@@ -6075,7 +6074,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="277" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="277" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G277" s="1" t="s">
         <v>222</v>
       </c>
@@ -6092,7 +6091,7 @@
         <v>54.917999999999999</v>
       </c>
     </row>
-    <row r="280" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F280" t="s">
         <v>13</v>
       </c>
@@ -6106,7 +6105,7 @@
         <v>58.77</v>
       </c>
     </row>
-    <row r="281" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F281" t="s">
         <v>14</v>
       </c>
@@ -6126,7 +6125,7 @@
         <v>54.49</v>
       </c>
     </row>
-    <row r="282" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F282" t="s">
         <v>15</v>
       </c>
@@ -6146,7 +6145,7 @@
         <v>56.86</v>
       </c>
     </row>
-    <row r="283" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F283" t="s">
         <v>16</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>50.91</v>
       </c>
     </row>
-    <row r="284" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F284" t="s">
         <v>17</v>
       </c>
@@ -6186,7 +6185,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="285" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F285" t="s">
         <v>18</v>
       </c>
@@ -6206,7 +6205,7 @@
         <v>50.33</v>
       </c>
     </row>
-    <row r="286" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F286" t="s">
         <v>19</v>
       </c>
@@ -6226,7 +6225,7 @@
         <v>50.71</v>
       </c>
     </row>
-    <row r="287" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F287" t="s">
         <v>20</v>
       </c>
@@ -6246,7 +6245,7 @@
         <v>50.78</v>
       </c>
     </row>
-    <row r="288" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F288" t="s">
         <v>21</v>
       </c>
@@ -6266,7 +6265,7 @@
         <v>50.08</v>
       </c>
     </row>
-    <row r="289" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F289" t="s">
         <v>22</v>
       </c>
@@ -6286,7 +6285,7 @@
         <v>50.4</v>
       </c>
     </row>
-    <row r="290" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="290" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G290" s="1" t="s">
         <v>222</v>
       </c>
@@ -6303,7 +6302,7 @@
         <v>100.568</v>
       </c>
     </row>
-    <row r="293" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="293" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F293" t="s">
         <v>13</v>
       </c>
@@ -6317,7 +6316,7 @@
         <v>82.41</v>
       </c>
     </row>
-    <row r="294" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="294" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F294" t="s">
         <v>14</v>
       </c>
@@ -6337,7 +6336,7 @@
         <v>68.569999999999993</v>
       </c>
     </row>
-    <row r="295" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F295" t="s">
         <v>15</v>
       </c>
@@ -6357,7 +6356,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="296" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F296" t="s">
         <v>16</v>
       </c>
@@ -6377,7 +6376,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="297" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F297" t="s">
         <v>17</v>
       </c>
@@ -6397,7 +6396,7 @@
         <v>71.150000000000006</v>
       </c>
     </row>
-    <row r="298" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F298" t="s">
         <v>18</v>
       </c>
@@ -6417,7 +6416,7 @@
         <v>68.41</v>
       </c>
     </row>
-    <row r="299" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="299" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F299" t="s">
         <v>19</v>
       </c>
@@ -6437,7 +6436,7 @@
         <v>73.31</v>
       </c>
     </row>
-    <row r="300" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F300" t="s">
         <v>20</v>
       </c>
@@ -6457,7 +6456,7 @@
         <v>68.39</v>
       </c>
     </row>
-    <row r="301" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="301" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F301" t="s">
         <v>21</v>
       </c>
@@ -6477,7 +6476,7 @@
         <v>70.77</v>
       </c>
     </row>
-    <row r="302" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="302" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F302" t="s">
         <v>22</v>
       </c>
@@ -6497,7 +6496,7 @@
         <v>64.47</v>
       </c>
     </row>
-    <row r="303" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="303" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G303" s="1" t="s">
         <v>222</v>
       </c>
@@ -6514,8 +6513,8 @@
         <v>119.82</v>
       </c>
     </row>
-    <row r="305" spans="6:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="G305" s="6" t="s">
+    <row r="305" spans="6:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G305" s="5" t="s">
         <v>249</v>
       </c>
       <c r="N305" s="1"/>
@@ -6525,7 +6524,7 @@
       <c r="R305" s="1"/>
       <c r="S305" s="1"/>
     </row>
-    <row r="306" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="306" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F306" t="s">
         <v>13</v>
       </c>
@@ -6540,7 +6539,7 @@
       </c>
       <c r="O306" s="4"/>
     </row>
-    <row r="307" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="307" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F307" t="s">
         <v>14</v>
       </c>
@@ -6561,7 +6560,7 @@
       </c>
       <c r="O307" s="4"/>
     </row>
-    <row r="308" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="308" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F308" t="s">
         <v>15</v>
       </c>
@@ -6582,7 +6581,7 @@
       </c>
       <c r="O308" s="4"/>
     </row>
-    <row r="309" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="309" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F309" t="s">
         <v>16</v>
       </c>
@@ -6603,7 +6602,7 @@
       </c>
       <c r="O309" s="4"/>
     </row>
-    <row r="310" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="310" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F310" t="s">
         <v>17</v>
       </c>
@@ -6624,7 +6623,7 @@
       </c>
       <c r="O310" s="4"/>
     </row>
-    <row r="311" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="311" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F311" t="s">
         <v>18</v>
       </c>
@@ -6645,7 +6644,7 @@
       </c>
       <c r="O311" s="4"/>
     </row>
-    <row r="312" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="312" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F312" t="s">
         <v>19</v>
       </c>
@@ -6666,7 +6665,7 @@
       </c>
       <c r="O312" s="4"/>
     </row>
-    <row r="313" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="313" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F313" t="s">
         <v>20</v>
       </c>
@@ -6687,7 +6686,7 @@
       </c>
       <c r="O313" s="4"/>
     </row>
-    <row r="314" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="314" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F314" t="s">
         <v>21</v>
       </c>
@@ -6708,7 +6707,7 @@
       </c>
       <c r="O314" s="4"/>
     </row>
-    <row r="315" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="315" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F315" t="s">
         <v>22</v>
       </c>
@@ -6729,7 +6728,7 @@
       </c>
       <c r="O315" s="4"/>
     </row>
-    <row r="316" spans="6:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="316" spans="6:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G316" s="1" t="s">
         <v>222</v>
       </c>
@@ -6747,12 +6746,12 @@
       </c>
       <c r="O316" s="1"/>
     </row>
-    <row r="318" spans="6:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="G318" s="6" t="s">
+    <row r="318" spans="6:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G318" s="5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="319" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="319" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F319" t="s">
         <v>13</v>
       </c>
@@ -6766,7 +6765,7 @@
         <v>6.23</v>
       </c>
     </row>
-    <row r="320" spans="6:19" x14ac:dyDescent="0.3">
+    <row r="320" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F320" t="s">
         <v>14</v>
       </c>
@@ -6786,7 +6785,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="321" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="321" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F321" t="s">
         <v>15</v>
       </c>
@@ -6806,7 +6805,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="322" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="322" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F322" t="s">
         <v>16</v>
       </c>
@@ -6826,7 +6825,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="323" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="323" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F323" t="s">
         <v>17</v>
       </c>
@@ -6846,7 +6845,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="324" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="324" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F324" t="s">
         <v>18</v>
       </c>
@@ -6866,7 +6865,7 @@
         <v>5.96</v>
       </c>
     </row>
-    <row r="325" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="325" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F325" t="s">
         <v>19</v>
       </c>
@@ -6886,7 +6885,7 @@
         <v>6.13</v>
       </c>
     </row>
-    <row r="326" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="326" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F326" t="s">
         <v>20</v>
       </c>
@@ -6906,7 +6905,7 @@
         <v>6.51</v>
       </c>
     </row>
-    <row r="327" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="327" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F327" t="s">
         <v>21</v>
       </c>
@@ -6926,7 +6925,7 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="328" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="328" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F328" t="s">
         <v>22</v>
       </c>
@@ -6946,7 +6945,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="329" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="329" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G329" s="1" t="s">
         <v>222</v>
       </c>
@@ -6963,7 +6962,7 @@
         <v>15.556000000000001</v>
       </c>
     </row>
-    <row r="332" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="332" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F332" t="s">
         <v>13</v>
       </c>
@@ -6977,7 +6976,7 @@
         <v>58.82</v>
       </c>
     </row>
-    <row r="333" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="333" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F333" t="s">
         <v>14</v>
       </c>
@@ -6997,7 +6996,7 @@
         <v>50.89</v>
       </c>
     </row>
-    <row r="334" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="334" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F334" t="s">
         <v>15</v>
       </c>
@@ -7017,7 +7016,7 @@
         <v>52.63</v>
       </c>
     </row>
-    <row r="335" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="335" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F335" t="s">
         <v>16</v>
       </c>
@@ -7037,7 +7036,7 @@
         <v>49.6</v>
       </c>
     </row>
-    <row r="336" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="336" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F336" t="s">
         <v>17</v>
       </c>
@@ -7057,7 +7056,7 @@
         <v>50.59</v>
       </c>
     </row>
-    <row r="337" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="337" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F337" t="s">
         <v>18</v>
       </c>
@@ -7077,7 +7076,7 @@
         <v>49.35</v>
       </c>
     </row>
-    <row r="338" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="338" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F338" t="s">
         <v>19</v>
       </c>
@@ -7097,7 +7096,7 @@
         <v>51.23</v>
       </c>
     </row>
-    <row r="339" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="339" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F339" t="s">
         <v>20</v>
       </c>
@@ -7117,7 +7116,7 @@
         <v>50.31</v>
       </c>
     </row>
-    <row r="340" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="340" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F340" t="s">
         <v>21</v>
       </c>
@@ -7137,7 +7136,7 @@
         <v>50.63</v>
       </c>
     </row>
-    <row r="341" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="341" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F341" t="s">
         <v>22</v>
       </c>
@@ -7157,7 +7156,7 @@
         <v>49.78</v>
       </c>
     </row>
-    <row r="342" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="342" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G342" s="1" t="s">
         <v>222</v>
       </c>
@@ -7174,7 +7173,7 @@
         <v>60.725999999999999</v>
       </c>
     </row>
-    <row r="345" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="345" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F345" t="s">
         <v>13</v>
       </c>
@@ -7188,7 +7187,7 @@
         <v>82.1</v>
       </c>
     </row>
-    <row r="346" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="346" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F346" t="s">
         <v>14</v>
       </c>
@@ -7208,7 +7207,7 @@
         <v>72.319999999999993</v>
       </c>
     </row>
-    <row r="347" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="347" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F347" t="s">
         <v>15</v>
       </c>
@@ -7228,7 +7227,7 @@
         <v>83.1</v>
       </c>
     </row>
-    <row r="348" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="348" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F348" t="s">
         <v>16</v>
       </c>
@@ -7248,7 +7247,7 @@
         <v>74.64</v>
       </c>
     </row>
-    <row r="349" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="349" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F349" t="s">
         <v>17</v>
       </c>
@@ -7268,7 +7267,7 @@
         <v>73.040000000000006</v>
       </c>
     </row>
-    <row r="350" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="350" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F350" t="s">
         <v>18</v>
       </c>
@@ -7288,7 +7287,7 @@
         <v>77.38</v>
       </c>
     </row>
-    <row r="351" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="351" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F351" t="s">
         <v>19</v>
       </c>
@@ -7308,7 +7307,7 @@
         <v>79.849999999999994</v>
       </c>
     </row>
-    <row r="352" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="352" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F352" t="s">
         <v>20</v>
       </c>
@@ -7328,7 +7327,7 @@
         <v>86.64</v>
       </c>
     </row>
-    <row r="353" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="353" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F353" t="s">
         <v>21</v>
       </c>
@@ -7348,7 +7347,7 @@
         <v>92.08</v>
       </c>
     </row>
-    <row r="354" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="354" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F354" t="s">
         <v>22</v>
       </c>
@@ -7368,7 +7367,7 @@
         <v>80.739999999999995</v>
       </c>
     </row>
-    <row r="355" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="355" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G355" s="1" t="s">
         <v>222</v>
       </c>
@@ -7385,7 +7384,7 @@
         <v>89.063999999999993</v>
       </c>
     </row>
-    <row r="358" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="358" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F358" t="s">
         <v>13</v>
       </c>
@@ -7399,7 +7398,7 @@
         <v>99.94</v>
       </c>
     </row>
-    <row r="359" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="359" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F359" t="s">
         <v>14</v>
       </c>
@@ -7419,7 +7418,7 @@
         <v>90.18</v>
       </c>
     </row>
-    <row r="360" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="360" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F360" t="s">
         <v>15</v>
       </c>
@@ -7439,7 +7438,7 @@
         <v>95.94</v>
       </c>
     </row>
-    <row r="361" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="361" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F361" t="s">
         <v>16</v>
       </c>
@@ -7459,7 +7458,7 @@
         <v>92.05</v>
       </c>
     </row>
-    <row r="362" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="362" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F362" t="s">
         <v>17</v>
       </c>
@@ -7479,7 +7478,7 @@
         <v>97.65</v>
       </c>
     </row>
-    <row r="363" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="363" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F363" t="s">
         <v>18</v>
       </c>
@@ -7499,7 +7498,7 @@
         <v>103.37</v>
       </c>
     </row>
-    <row r="364" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="364" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F364" t="s">
         <v>19</v>
       </c>
@@ -7519,7 +7518,7 @@
         <v>98.67</v>
       </c>
     </row>
-    <row r="365" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="365" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F365" t="s">
         <v>20</v>
       </c>
@@ -7539,7 +7538,7 @@
         <v>103.83</v>
       </c>
     </row>
-    <row r="366" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="366" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F366" t="s">
         <v>21</v>
       </c>
@@ -7559,7 +7558,7 @@
         <v>101.89</v>
       </c>
     </row>
-    <row r="367" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="367" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F367" t="s">
         <v>22</v>
       </c>
@@ -7579,7 +7578,7 @@
         <v>99.24</v>
       </c>
     </row>
-    <row r="368" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="368" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G368" s="1" t="s">
         <v>222</v>
       </c>
@@ -7596,7 +7595,7 @@
         <v>210.34199999999998</v>
       </c>
     </row>
-    <row r="371" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="371" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F371" t="s">
         <v>13</v>
       </c>
@@ -7610,7 +7609,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="372" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="372" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F372" t="s">
         <v>14</v>
       </c>
@@ -7630,7 +7629,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="373" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="373" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F373" t="s">
         <v>15</v>
       </c>
@@ -7650,7 +7649,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="374" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="374" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F374" t="s">
         <v>16</v>
       </c>
@@ -7670,7 +7669,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="375" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="375" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F375" t="s">
         <v>17</v>
       </c>
@@ -7690,7 +7689,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="376" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="376" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F376" t="s">
         <v>18</v>
       </c>
@@ -7710,7 +7709,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="377" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="377" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F377" t="s">
         <v>19</v>
       </c>
@@ -7730,7 +7729,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="378" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="378" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F378" t="s">
         <v>20</v>
       </c>
@@ -7750,7 +7749,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="379" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="379" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F379" t="s">
         <v>21</v>
       </c>
@@ -7770,7 +7769,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="380" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="380" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F380" t="s">
         <v>22</v>
       </c>
@@ -7790,7 +7789,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="381" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="381" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G381" s="1" t="s">
         <v>222</v>
       </c>
@@ -7807,7 +7806,7 @@
         <v>160.53399999999999</v>
       </c>
     </row>
-    <row r="384" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="384" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F384" t="s">
         <v>13</v>
       </c>
@@ -7821,7 +7820,7 @@
         <v>50.49</v>
       </c>
     </row>
-    <row r="385" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="385" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F385" t="s">
         <v>14</v>
       </c>
@@ -7841,7 +7840,7 @@
         <v>47.46</v>
       </c>
     </row>
-    <row r="386" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="386" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F386" t="s">
         <v>15</v>
       </c>
@@ -7861,7 +7860,7 @@
         <v>50.7</v>
       </c>
     </row>
-    <row r="387" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="387" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F387" t="s">
         <v>16</v>
       </c>
@@ -7881,7 +7880,7 @@
         <v>52.17</v>
       </c>
     </row>
-    <row r="388" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="388" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F388" t="s">
         <v>17</v>
       </c>
@@ -7901,7 +7900,7 @@
         <v>51.27</v>
       </c>
     </row>
-    <row r="389" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="389" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F389" t="s">
         <v>18</v>
       </c>
@@ -7921,7 +7920,7 @@
         <v>50.76</v>
       </c>
     </row>
-    <row r="390" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="390" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F390" t="s">
         <v>19</v>
       </c>
@@ -7941,7 +7940,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="391" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="391" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F391" t="s">
         <v>20</v>
       </c>
@@ -7961,7 +7960,7 @@
         <v>50.73</v>
       </c>
     </row>
-    <row r="392" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="392" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F392" t="s">
         <v>21</v>
       </c>
@@ -7981,7 +7980,7 @@
         <v>50.63</v>
       </c>
     </row>
-    <row r="393" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="393" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F393" t="s">
         <v>22</v>
       </c>
@@ -8001,7 +8000,7 @@
         <v>50.68</v>
       </c>
     </row>
-    <row r="394" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="394" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G394" s="1" t="s">
         <v>222</v>
       </c>
@@ -8018,7 +8017,7 @@
         <v>210.38599999999997</v>
       </c>
     </row>
-    <row r="397" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="397" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F397" t="s">
         <v>13</v>
       </c>
@@ -8032,7 +8031,7 @@
         <v>118.3</v>
       </c>
     </row>
-    <row r="398" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="398" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F398" t="s">
         <v>14</v>
       </c>
@@ -8052,7 +8051,7 @@
         <v>89.29</v>
       </c>
     </row>
-    <row r="399" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="399" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F399" t="s">
         <v>15</v>
       </c>
@@ -8072,7 +8071,7 @@
         <v>89.8</v>
       </c>
     </row>
-    <row r="400" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="400" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F400" t="s">
         <v>16</v>
       </c>
@@ -8092,7 +8091,7 @@
         <v>91.54</v>
       </c>
     </row>
-    <row r="401" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="401" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F401" t="s">
         <v>17</v>
       </c>
@@ -8112,7 +8111,7 @@
         <v>90.23</v>
       </c>
     </row>
-    <row r="402" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="402" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F402" t="s">
         <v>18</v>
       </c>
@@ -8132,7 +8131,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="403" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="403" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F403" t="s">
         <v>19</v>
       </c>
@@ -8152,7 +8151,7 @@
         <v>92.47</v>
       </c>
     </row>
-    <row r="404" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="404" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F404" t="s">
         <v>20</v>
       </c>
@@ -8172,7 +8171,7 @@
         <v>90.08</v>
       </c>
     </row>
-    <row r="405" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="405" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F405" t="s">
         <v>21</v>
       </c>
@@ -8192,7 +8191,7 @@
         <v>93.74</v>
       </c>
     </row>
-    <row r="406" spans="6:12" x14ac:dyDescent="0.3">
+    <row r="406" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F406" t="s">
         <v>22</v>
       </c>
@@ -8212,7 +8211,7 @@
         <v>91.59</v>
       </c>
     </row>
-    <row r="407" spans="6:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="407" spans="6:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G407" s="1" t="s">
         <v>222</v>
       </c>

</xml_diff>